<commit_message>
modificando os artefatos 15, 16, 17, 18 conforme o mostrado pelo professor
</commit_message>
<xml_diff>
--- a/17 - Descrição dos Processos de Negócios.xlsx
+++ b/17 - Descrição dos Processos de Negócios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8cd3af5bce398e7e/ADS/terceiroSemestre/engenharia_de_requisitos/ACS/AC3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{F634FC32-32F0-4C01-93FA-26A114ED05F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{855D420A-4B85-4CB7-8347-43BF22DB053D}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{F634FC32-32F0-4C01-93FA-26A114ED05F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B7948881-9DE4-4B22-9339-1480CEA525F4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB4E0864-EB05-4810-AA47-D6EDDC1DA012}"/>
+    <workbookView xWindow="4515" yWindow="2985" windowWidth="23265" windowHeight="11385" xr2:uid="{CB4E0864-EB05-4810-AA47-D6EDDC1DA012}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Capacidades</t>
   </si>
@@ -231,10 +231,16 @@
     <t>Cliente realiza pagamento com dinheiro</t>
   </si>
   <si>
-    <t>Cliente realiza pagamento com Cartão de Crédito / Débito</t>
-  </si>
-  <si>
     <t>x(1)</t>
+  </si>
+  <si>
+    <t>Cliente Efetua o pagamento em cartão</t>
+  </si>
+  <si>
+    <t>Provedor de cartão envia resposta</t>
+  </si>
+  <si>
+    <t>x(3)</t>
   </si>
 </sst>
 </file>
@@ -271,7 +277,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,8 +338,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -505,14 +523,16 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
         <color indexed="64"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -523,7 +543,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -531,11 +553,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -599,52 +634,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -658,23 +647,99 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,7 +1064,7 @@
   <dimension ref="A3:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,22 +1081,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="40"/>
+      <c r="G3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="27" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1057,204 +1122,247 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="35">
         <v>1</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="42"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="39">
+      <c r="A6" s="43"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="35">
         <v>2</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42"/>
+      <c r="E6" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="39">
-        <v>3</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="42"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="J10" s="39"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="J11" s="39"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="J12" s="39"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="23">
+        <v>3</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="37"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="J13" s="39"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="23">
+        <v>4</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="37"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
+      <c r="J14" s="39"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="38"/>
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
+      <c r="J15" s="39"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="J16" s="39"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="38"/>
       <c r="H17" s="38"/>
       <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
+      <c r="J17" s="39"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:A17"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B13:B17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1273,25 +1381,25 @@
   <sheetData>
     <row r="5" spans="3:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="24" t="s">
+      <c r="D5" s="59"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="24" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="26"/>
-      <c r="K5" s="25"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="49"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="3:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1321,7 +1429,7 @@
       <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="53" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="10">
@@ -1343,7 +1451,7 @@
       <c r="C8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="54"/>
       <c r="E8" s="10">
         <v>2</v>
       </c>
@@ -1361,7 +1469,7 @@
     </row>
     <row r="9" spans="3:12" ht="75" x14ac:dyDescent="0.25">
       <c r="C9" s="8"/>
-      <c r="D9" s="30"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="10">
         <v>3</v>
       </c>
@@ -1379,7 +1487,7 @@
     </row>
     <row r="10" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="8"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="54"/>
       <c r="E10" s="10">
         <v>4</v>
       </c>
@@ -1397,7 +1505,7 @@
     </row>
     <row r="11" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="8"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="10">
         <v>5</v>
       </c>
@@ -1415,7 +1523,7 @@
     </row>
     <row r="12" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="8"/>
-      <c r="D12" s="31"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="10">
         <v>6</v>
       </c>
@@ -1433,7 +1541,7 @@
     </row>
     <row r="13" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C13" s="8"/>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="53" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="10">
@@ -1453,7 +1561,7 @@
     </row>
     <row r="14" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="10">
         <v>8</v>
       </c>
@@ -1471,7 +1579,7 @@
     </row>
     <row r="15" spans="3:12" ht="90" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
-      <c r="D15" s="31"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="10">
         <v>9</v>
       </c>
@@ -1491,7 +1599,7 @@
       <c r="C16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="53" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="10">
@@ -1513,7 +1621,7 @@
       <c r="C17" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="31"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="10">
         <v>11</v>
       </c>
@@ -1531,7 +1639,7 @@
     </row>
     <row r="18" spans="3:12" ht="75" x14ac:dyDescent="0.25">
       <c r="C18" s="18"/>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="53" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="10">
@@ -1551,7 +1659,7 @@
     </row>
     <row r="19" spans="3:12" ht="60" x14ac:dyDescent="0.25">
       <c r="C19" s="19"/>
-      <c r="D19" s="31"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="10">
         <v>13</v>
       </c>
@@ -1568,7 +1676,7 @@
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="56" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="20" t="s">
@@ -1590,8 +1698,8 @@
       </c>
     </row>
     <row r="21" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C21" s="33"/>
-      <c r="D21" s="29" t="s">
+      <c r="C21" s="57"/>
+      <c r="D21" s="53" t="s">
         <v>48</v>
       </c>
       <c r="E21" s="10">
@@ -1610,8 +1718,8 @@
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="3:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="C22" s="34"/>
-      <c r="D22" s="31"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="10">
         <v>16</v>
       </c>

</xml_diff>